<commit_message>
Alpha teste sabe como é
</commit_message>
<xml_diff>
--- a/usuarios.xlsx
+++ b/usuarios.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Sistema-Automatizado-de-Teatro\"/>
     </mc:Choice>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>Nome</t>
   </si>
@@ -42,12 +42,22 @@
   </si>
   <si>
     <t>123</t>
+  </si>
+  <si>
+    <t>Angelo</t>
+  </si>
+  <si>
+    <t>96655682215</t>
+  </si>
+  <si>
+    <t>03/02/2005</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -393,7 +403,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F6" sqref="A1:XFD1048576"/>
@@ -401,9 +411,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.81640625"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -453,36 +481,36 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>5</v>
       </c>
     </row>

</xml_diff>